<commit_message>
base finished chapter 8 100%
</commit_message>
<xml_diff>
--- a/autocrword/models/wind_f/工程量表/电气工程量表-zyc.xlsx
+++ b/autocrword/models/wind_f/工程量表/电气工程量表-zyc.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EFA382C-394D-4E7B-A8EC-0CDDF1B1D86C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39856725-0B50-477F-80B5-5A8793A5D947}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="2370" windowWidth="20670" windowHeight="12795" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1770" windowWidth="27885" windowHeight="13830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="箱变容量选型表" sheetId="1" r:id="rId1"/>
@@ -1527,6 +1527,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1546,7 +1614,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACE"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>

</xml_diff>